<commit_message>
Make Fuction to Goto SubSbuNavbar using Text Field, and Create SCD0171 - Menu BNI Multi Finance
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0170_Buka BNI Multifinance.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0170_Buka BNI Multifinance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA94510-AECC-43AD-B778-FD53FC5EC76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246B453C-BD4F-4BAF-9CE7-0E7A0C18F56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="3615" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0170" sheetId="2" r:id="rId1"/>
@@ -87,10 +87,10 @@
     <t>Terdapat penambahan Menu BNI Multifinance</t>
   </si>
   <si>
-    <t>Lihat Semua</t>
-  </si>
-  <si>
     <t>· Login pada aplikasi digisales dengan menggunakan user Sales</t>
+  </si>
+  <si>
+    <t>BNI Multi Finance</t>
   </si>
 </sst>
 </file>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>16</v>
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="13"/>

</xml_diff>

<commit_message>
Regretion SCD0187 and SCD0191. Then Update Excel SCD0170 - SCD0187
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0170_Buka BNI Multifinance.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0170_Buka BNI Multifinance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246B453C-BD4F-4BAF-9CE7-0E7A0C18F56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2AEC1E-C7C3-458A-91FD-4305E9C8CA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="3615" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0170" sheetId="2" r:id="rId1"/>
@@ -492,7 +492,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,9 +506,8 @@
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>

</xml_diff>